<commit_message>
Linklist.c  When will *head value be changed?
</commit_message>
<xml_diff>
--- a/interview/interviewPlan.xlsx
+++ b/interview/interviewPlan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>epoll</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>settimer</t>
+  </si>
+  <si>
+    <t>linklist</t>
+  </si>
+  <si>
+    <t>merge 2 linklists without using the third linklist</t>
+  </si>
+  <si>
+    <t>doing the practice</t>
   </si>
 </sst>
 </file>
@@ -52,12 +61,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -72,8 +87,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -354,14 +370,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:D8"/>
+  <dimension ref="B1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
+    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>2</v>
@@ -388,6 +410,14 @@
     <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D8" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
char *str[5] vs char (*str)[5]
</commit_message>
<xml_diff>
--- a/interview/interviewPlan.xlsx
+++ b/interview/interviewPlan.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>epoll</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>doing the practice</t>
+  </si>
+  <si>
+    <t>memory leak</t>
+  </si>
+  <si>
+    <t>valgrind</t>
+  </si>
+  <si>
+    <t>arm assemble</t>
   </si>
 </sst>
 </file>
@@ -370,10 +379,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D9"/>
+  <dimension ref="B1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -420,6 +429,19 @@
         <v>7</v>
       </c>
     </row>
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>